<commit_message>
Supplementary material for internal review
</commit_message>
<xml_diff>
--- a/supplementary-material/inputs/prisma.xlsx
+++ b/supplementary-material/inputs/prisma.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davetaylor/dev/transitions-review/supplementary-material/inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dtay0016/dev/youth-homelessness-review/supplementary-material/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D0399B1-6964-7C4E-A3BE-1F09199217D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B13D295F-439E-0B43-916E-5A517FAA0F11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{A1839663-239A-1A4B-89C5-AE8F063D74BB}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="17520" xr2:uid="{A1839663-239A-1A4B-89C5-AE8F063D74BB}"/>
   </bookViews>
   <sheets>
     <sheet name="prisma" sheetId="21" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="124">
   <si>
     <t xml:space="preserve">Section and Topic </t>
   </si>
@@ -375,33 +375,9 @@
     <t>In section: "Search Methods"</t>
   </si>
   <si>
-    <t xml:space="preserve">Provided in discussion of results for each outcome. Additional detail for GRADE assessment provided in supplementary material. </t>
-  </si>
-  <si>
-    <t>Provided in sections: "Main results for transitions support programs" and "Main results for extended care policies"</t>
-  </si>
-  <si>
     <t>Provided in section: "Conclusion"</t>
   </si>
   <si>
-    <t>Provided in Figure 3 and Figure 4.</t>
-  </si>
-  <si>
-    <t>Provided in Tables 2, 3, 4, 5, 5, 6, 7, 8 &amp; 9</t>
-  </si>
-  <si>
-    <t>Provided in discussion of results for each outcome and Figures 5 &amp; 6.</t>
-  </si>
-  <si>
-    <t>Provided in section "Subgroup and sensitivity analysis"</t>
-  </si>
-  <si>
-    <t>Provided in Table 1.</t>
-  </si>
-  <si>
-    <t>Provided in Figure 2.</t>
-  </si>
-  <si>
     <t>Provided in "Implications for research"</t>
   </si>
   <si>
@@ -412,6 +388,27 @@
   </si>
   <si>
     <t>Discussion</t>
+  </si>
+  <si>
+    <t>Provided in Figure 1.</t>
+  </si>
+  <si>
+    <t>Provided in Table 2.</t>
+  </si>
+  <si>
+    <t>Provided in Figure 2 and Figure 3.</t>
+  </si>
+  <si>
+    <t>Not applicable</t>
+  </si>
+  <si>
+    <t>Provided in Tables 4, 5, 6, 7, 8, 9,10 &amp; 11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Provided in discussion of results for each outcome. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Provided in sections: "Main results" </t>
   </si>
 </sst>
 </file>
@@ -721,6 +718,24 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -729,24 +744,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -766,9 +763,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -806,7 +803,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -912,7 +909,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1054,7 +1051,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1067,8 +1064,8 @@
   </sheetPr>
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1132,7 +1129,7 @@
         <v>9</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1418,11 +1415,11 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="18"/>
-      <c r="C27" s="19"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="25"/>
       <c r="D27" s="13"/>
     </row>
     <row r="28" spans="1:4" ht="53" thickBot="1" x14ac:dyDescent="0.25">
@@ -1436,7 +1433,7 @@
         <v>55</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="40" thickBot="1" x14ac:dyDescent="0.25">
@@ -1449,8 +1446,8 @@
       <c r="C29" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="D29" s="23" t="s">
-        <v>103</v>
+      <c r="D29" s="17" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="40" thickBot="1" x14ac:dyDescent="0.25">
@@ -1464,7 +1461,7 @@
         <v>59</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.25">
@@ -1478,7 +1475,7 @@
         <v>61</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="66" thickBot="1" x14ac:dyDescent="0.25">
@@ -1492,7 +1489,7 @@
         <v>63</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="40" thickBot="1" x14ac:dyDescent="0.25">
@@ -1506,7 +1503,7 @@
         <v>66</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="79" thickBot="1" x14ac:dyDescent="0.25">
@@ -1520,7 +1517,7 @@
         <v>68</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.25">
@@ -1534,7 +1531,7 @@
         <v>70</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>103</v>
+        <v>120</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="40" thickBot="1" x14ac:dyDescent="0.25">
@@ -1548,7 +1545,7 @@
         <v>72</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="40" thickBot="1" x14ac:dyDescent="0.25">
@@ -1576,20 +1573,20 @@
         <v>76</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="17" t="s">
+      <c r="A39" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="B39" s="18"/>
-      <c r="C39" s="19"/>
+      <c r="B39" s="24"/>
+      <c r="C39" s="25"/>
       <c r="D39" s="13"/>
     </row>
-    <row r="40" spans="1:4" ht="40" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="25" t="s">
-        <v>124</v>
+    <row r="40" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="19" t="s">
+        <v>116</v>
       </c>
       <c r="B40" s="10" t="s">
         <v>78</v>
@@ -1597,13 +1594,13 @@
       <c r="C40" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="D40" s="12" t="s">
-        <v>113</v>
+      <c r="D40" s="18" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="25" t="s">
-        <v>124</v>
+      <c r="A41" s="19" t="s">
+        <v>116</v>
       </c>
       <c r="B41" s="10" t="s">
         <v>80</v>
@@ -1612,12 +1609,12 @@
         <v>81</v>
       </c>
       <c r="D41" s="12" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="25" t="s">
-        <v>124</v>
+      <c r="A42" s="19" t="s">
+        <v>116</v>
       </c>
       <c r="B42" s="14" t="s">
         <v>82</v>
@@ -1626,7 +1623,7 @@
         <v>83</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1686,11 +1683,11 @@
       <c r="B47" s="10">
         <v>25</v>
       </c>
-      <c r="C47" s="24" t="s">
+      <c r="C47" s="18" t="s">
         <v>93</v>
       </c>
       <c r="D47" s="12" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.25">
@@ -1700,11 +1697,11 @@
       <c r="B48" s="10">
         <v>26</v>
       </c>
-      <c r="C48" s="24" t="s">
+      <c r="C48" s="18" t="s">
         <v>95</v>
       </c>
       <c r="D48" s="12" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="66" thickBot="1" x14ac:dyDescent="0.25">
@@ -1714,7 +1711,7 @@
       <c r="B49" s="16">
         <v>27</v>
       </c>
-      <c r="C49" s="23" t="s">
+      <c r="C49" s="17" t="s">
         <v>97</v>
       </c>
       <c r="D49" s="8" t="s">
@@ -1724,13 +1721,13 @@
     <row r="50" spans="1:4" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="A43:C43"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="A9:C9"/>
     <mergeCell ref="A27:C27"/>
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="A43:C43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>